<commit_message>
Small changes, implemented mass
</commit_message>
<xml_diff>
--- a/Output2.xlsx
+++ b/Output2.xlsx
@@ -546,64 +546,64 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5676.999999999993</v>
+        <v>406.7620641209767</v>
       </c>
       <c r="C2">
-        <v>9023.000000000011</v>
+        <v>1423.784512505422</v>
       </c>
       <c r="D2">
-        <v>23050</v>
+        <v>1826.697150462707</v>
       </c>
       <c r="E2">
-        <v>734.1999999999997</v>
+        <v>64.62950279638585</v>
       </c>
       <c r="F2">
-        <v>415.1000000000009</v>
+        <v>19.42673116764596</v>
       </c>
       <c r="G2">
-        <v>4098.800000000005</v>
+        <v>307.1297081676828</v>
       </c>
       <c r="H2">
-        <v>1173</v>
+        <v>26.3382283904123</v>
       </c>
       <c r="I2">
-        <v>18629.5</v>
+        <v>688.7475634103021</v>
       </c>
       <c r="J2">
-        <v>1252.54</v>
+        <v>16.35272369515465</v>
       </c>
       <c r="K2">
-        <v>175.5300000000001</v>
+        <v>5.513404951952301</v>
       </c>
       <c r="L2">
-        <v>4648.499999999999</v>
+        <v>117.8835876429822</v>
       </c>
       <c r="M2">
-        <v>25.51800000000003</v>
+        <v>1.221204087471981</v>
       </c>
       <c r="N2">
-        <v>13.104</v>
+        <v>1.006854132101349</v>
       </c>
       <c r="O2">
-        <v>201.7749999999999</v>
+        <v>13.39270749288584</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>1186.6</v>
+        <v>64.72721744196113</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>1186.6</v>
+        <v>64.72721744196113</v>
       </c>
       <c r="T2">
-        <v>1186.6</v>
+        <v>64.72721744196113</v>
       </c>
       <c r="U2">
-        <v>2.81</v>
+        <v>1.633954832474227</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>111788.7</v>
+        <v>1131.535015516773</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -629,64 +629,64 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>5027.899999999997</v>
+        <v>17861.818533069</v>
       </c>
       <c r="C3">
-        <v>7772.100000000009</v>
+        <v>124276.8874610486</v>
       </c>
       <c r="D3">
-        <v>20733</v>
+        <v>95598.60442291811</v>
       </c>
       <c r="E3">
-        <v>645.5</v>
+        <v>4533.759471289621</v>
       </c>
       <c r="F3">
-        <v>394.2000000000006</v>
+        <v>5762.283039516643</v>
       </c>
       <c r="G3">
-        <v>3652.100000000004</v>
+        <v>6432.12558334999</v>
       </c>
       <c r="H3">
-        <v>937</v>
+        <v>17.00465880233554</v>
       </c>
       <c r="I3">
-        <v>16520</v>
+        <v>168683.7684859641</v>
       </c>
       <c r="J3">
-        <v>940.6399999999998</v>
+        <v>292.2271643795879</v>
       </c>
       <c r="K3">
-        <v>151.76</v>
+        <v>4.255912753998186</v>
       </c>
       <c r="L3">
-        <v>3776.199999999999</v>
+        <v>2472.298894748137</v>
       </c>
       <c r="M3">
-        <v>23.40850000000001</v>
+        <v>64.04697408836569</v>
       </c>
       <c r="N3">
-        <v>11.79500000000001</v>
+        <v>267.0271231858534</v>
       </c>
       <c r="O3">
-        <v>179.3749999999999</v>
+        <v>151.3571743724798</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1118.8</v>
+        <v>11259.30068662367</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3">
-        <v>1118.8</v>
+        <v>11259.30068662367</v>
       </c>
       <c r="T3">
-        <v>1118.8</v>
+        <v>11259.30068662367</v>
       </c>
       <c r="U3">
-        <v>2.94</v>
+        <v>1.182775708762887</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>79664.25000000004</v>
+        <v>75058.96728275302</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -712,64 +712,64 @@
         <v>201</v>
       </c>
       <c r="B4">
-        <v>8012.099999999989</v>
+        <v>417.0983106078516</v>
       </c>
       <c r="C4">
-        <v>11087.90000000001</v>
+        <v>730.3517250623604</v>
       </c>
       <c r="D4">
-        <v>33241</v>
+        <v>1673.703985177697</v>
       </c>
       <c r="E4">
-        <v>1012.999999999999</v>
+        <v>70.05364113557339</v>
       </c>
       <c r="F4">
-        <v>721.1000000000009</v>
+        <v>12.32842606886002</v>
       </c>
       <c r="G4">
-        <v>5694.600000000001</v>
+        <v>321.2683864559366</v>
       </c>
       <c r="H4">
-        <v>1457</v>
+        <v>23.18353026380176</v>
       </c>
       <c r="I4">
-        <v>29669.5</v>
+        <v>463.6137425946026</v>
       </c>
       <c r="J4">
-        <v>1661.52</v>
+        <v>16.60971840232479</v>
       </c>
       <c r="K4">
-        <v>271.2499999999999</v>
+        <v>5.997600285112068</v>
       </c>
       <c r="L4">
-        <v>5500.5</v>
+        <v>116.8732224632952</v>
       </c>
       <c r="M4">
-        <v>35.67100000000005</v>
+        <v>1.250543040696576</v>
       </c>
       <c r="N4">
-        <v>17.743</v>
+        <v>0.7988417300089758</v>
       </c>
       <c r="O4">
-        <v>281.6149999999999</v>
+        <v>15.58366849701403</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>1924.400000000001</v>
+        <v>53.17998944211951</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>1924.400000000001</v>
+        <v>53.17998944211951</v>
       </c>
       <c r="T4">
-        <v>1924.400000000001</v>
+        <v>53.17998944211951</v>
       </c>
       <c r="U4">
-        <v>2.68</v>
+        <v>1.903133956185567</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>130328.15</v>
+        <v>1095.504932171302</v>
       </c>
       <c r="AA4">
         <v>0</v>
@@ -795,64 +795,64 @@
         <v>208</v>
       </c>
       <c r="B5">
-        <v>6328.799999999993</v>
+        <v>409.595483460815</v>
       </c>
       <c r="C5">
-        <v>9471.200000000004</v>
+        <v>1291.95929768566</v>
       </c>
       <c r="D5">
-        <v>26098</v>
+        <v>1740.755188175594</v>
       </c>
       <c r="E5">
-        <v>758.3999999999995</v>
+        <v>70.04260997750842</v>
       </c>
       <c r="F5">
-        <v>533.0000000000007</v>
+        <v>36.88105418043184</v>
       </c>
       <c r="G5">
-        <v>4596.000000000004</v>
+        <v>284.1467258585485</v>
       </c>
       <c r="H5">
-        <v>1038</v>
+        <v>19.26651188320137</v>
       </c>
       <c r="I5">
-        <v>21888</v>
+        <v>1277.309704408859</v>
       </c>
       <c r="J5">
-        <v>1243.1</v>
+        <v>14.39328545874083</v>
       </c>
       <c r="K5">
-        <v>184.96</v>
+        <v>3.979739452712001</v>
       </c>
       <c r="L5">
-        <v>4231.199999999999</v>
+        <v>92.2904584315487</v>
       </c>
       <c r="M5">
-        <v>26.16850000000003</v>
+        <v>1.16362985944985</v>
       </c>
       <c r="N5">
-        <v>14.259</v>
+        <v>1.769198074903962</v>
       </c>
       <c r="O5">
-        <v>204.6449999999999</v>
+        <v>11.200398795048</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>1481.800000000001</v>
+        <v>109.7489180334657</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>1481.800000000001</v>
+        <v>109.7489180334657</v>
       </c>
       <c r="T5">
-        <v>1481.800000000001</v>
+        <v>109.7489180334657</v>
       </c>
       <c r="U5">
-        <v>3.069999999999999</v>
+        <v>1.826277963917526</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>101028.7</v>
+        <v>1061.204673530374</v>
       </c>
       <c r="AA5">
         <v>0</v>

</xml_diff>

<commit_message>
Need to check output
</commit_message>
<xml_diff>
--- a/Output2.xlsx
+++ b/Output2.xlsx
@@ -564,10 +564,10 @@
         <v>307.1297081676828</v>
       </c>
       <c r="H2">
-        <v>26.3382283904123</v>
+        <v>26.33822839041229</v>
       </c>
       <c r="I2">
-        <v>688.7475634103021</v>
+        <v>688.747563410302</v>
       </c>
       <c r="J2">
         <v>16.35272369515465</v>
@@ -591,16 +591,16 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>64.72721744196113</v>
+        <v>64.72721744196112</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>64.72721744196113</v>
+        <v>64.72721744196112</v>
       </c>
       <c r="T2">
-        <v>64.72721744196113</v>
+        <v>64.72721744196112</v>
       </c>
       <c r="U2">
         <v>1.633954832474227</v>
@@ -659,7 +659,7 @@
         <v>4.255912753998186</v>
       </c>
       <c r="L3">
-        <v>2472.298894748137</v>
+        <v>2472.298894748136</v>
       </c>
       <c r="M3">
         <v>64.04697408836569</v>
@@ -757,16 +757,16 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>53.17998944211951</v>
+        <v>53.1799894421195</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>53.17998944211951</v>
+        <v>53.1799894421195</v>
       </c>
       <c r="T4">
-        <v>53.17998944211951</v>
+        <v>53.1799894421195</v>
       </c>
       <c r="U4">
         <v>1.903133956185567</v>
@@ -825,7 +825,7 @@
         <v>3.979739452712001</v>
       </c>
       <c r="L5">
-        <v>92.2904584315487</v>
+        <v>92.29045843154871</v>
       </c>
       <c r="M5">
         <v>1.16362985944985</v>

</xml_diff>